<commit_message>
Bolus Dosage Changes... need to work on thresholds
</commit_message>
<xml_diff>
--- a/data_analysis/PythonPipeline/Modules/Patient_9_Dosage.xlsx
+++ b/data_analysis/PythonPipeline/Modules/Patient_9_Dosage.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b14a0d7b62cf6ad0/Sid Stuff/PROJECTS/iMEDS Design Team/Data Analysis/PedAccel/data_analysis/PythonPipeline/Modules/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="21" documentId="8_{922AB683-9D13-4D32-93D7-B817AFC9F0AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2BD0A8A6-C45A-4409-BDF2-5BADD89C557F}"/>
+  <xr:revisionPtr revIDLastSave="49" documentId="8_{922AB683-9D13-4D32-93D7-B817AFC9F0AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{76E09BAC-4685-4D5F-A727-6D7DEE0CB07F}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14476" xr2:uid="{809031ED-8969-471B-B3A5-4615F6501142}"/>
   </bookViews>
@@ -683,8 +683,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D9BB840-B148-4D47-929F-444E835E0A98}">
   <dimension ref="A1:P142"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -749,6 +749,9 @@
         <f>TEXT(A4,"M/dd/yyyy hh:mm::ss AM/PM")</f>
         <v>1/15/2024  14:00:00 PM</v>
       </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
       <c r="M4">
         <v>0</v>
       </c>
@@ -794,6 +797,9 @@
         <f t="shared" si="0"/>
         <v>1/15/2024  15:42:00 PM</v>
       </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
       <c r="M6">
         <v>1</v>
       </c>
@@ -812,6 +818,9 @@
         <f t="shared" si="0"/>
         <v>1/15/2024  16:00:00 PM</v>
       </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
       <c r="I7">
         <v>0.39400000000000002</v>
       </c>
@@ -857,6 +866,9 @@
         <f t="shared" si="0"/>
         <v>1/15/2024  17:00:00 PM</v>
       </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
       <c r="I9">
         <v>0.39400000000000002</v>
       </c>
@@ -876,6 +888,9 @@
         <f t="shared" si="0"/>
         <v>1/15/2024  18:00:00 PM</v>
       </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
       <c r="I10">
         <v>0.39400000000000002</v>
       </c>
@@ -900,6 +915,9 @@
         <f t="shared" si="0"/>
         <v>1/15/2024  19:00:00 PM</v>
       </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
       <c r="I11">
         <v>0.39400000000000002</v>
       </c>
@@ -919,6 +937,9 @@
         <f t="shared" si="0"/>
         <v>1/15/2024  19:05:00 PM</v>
       </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
       <c r="E12" s="3"/>
       <c r="M12">
         <v>1</v>
@@ -962,6 +983,9 @@
         <f t="shared" si="0"/>
         <v>1/15/2024  20:00:00 PM</v>
       </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
       <c r="I14">
         <v>0.39400000000000002</v>
       </c>
@@ -986,6 +1010,9 @@
         <f t="shared" si="0"/>
         <v>1/15/2024  20:14:00 PM</v>
       </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
       <c r="M15">
         <v>1</v>
       </c>
@@ -1001,6 +1028,9 @@
         <f t="shared" si="0"/>
         <v>1/15/2024  20:28:00 PM</v>
       </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
       <c r="M16">
         <v>-1</v>
       </c>
@@ -1016,6 +1046,9 @@
         <f t="shared" si="0"/>
         <v>1/15/2024  21:00:00 PM</v>
       </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
       <c r="I17">
         <v>0.39400000000000002</v>
       </c>
@@ -1035,6 +1068,9 @@
         <f t="shared" si="0"/>
         <v>1/15/2024  22:00:00 PM</v>
       </c>
+      <c r="C18">
+        <v>0</v>
+      </c>
       <c r="I18">
         <v>0.39400000000000002</v>
       </c>
@@ -1054,6 +1090,9 @@
         <f t="shared" si="0"/>
         <v>1/15/2024  23:00:00 PM</v>
       </c>
+      <c r="C19">
+        <v>0</v>
+      </c>
       <c r="I19">
         <v>0.39400000000000002</v>
       </c>
@@ -1073,6 +1112,9 @@
         <f t="shared" si="0"/>
         <v>1/15/2024  23:50:00 PM</v>
       </c>
+      <c r="C20">
+        <v>0</v>
+      </c>
       <c r="M20">
         <v>1</v>
       </c>
@@ -1087,6 +1129,9 @@
       <c r="B21" s="14" t="str">
         <f t="shared" si="0"/>
         <v>1/16/2024 12:00:00 AM</v>
+      </c>
+      <c r="C21">
+        <v>0</v>
       </c>
       <c r="D21" s="12"/>
       <c r="E21" s="7"/>
@@ -1116,6 +1161,9 @@
         <f t="shared" si="0"/>
         <v>1/16/2024 01:00:00 AM</v>
       </c>
+      <c r="C22">
+        <v>0</v>
+      </c>
       <c r="I22">
         <v>0.39400000000000002</v>
       </c>
@@ -1135,6 +1183,9 @@
         <f t="shared" si="0"/>
         <v>1/16/2024 02:00:00 AM</v>
       </c>
+      <c r="C23">
+        <v>0</v>
+      </c>
       <c r="I23">
         <v>0.39400000000000002</v>
       </c>
@@ -1175,6 +1226,9 @@
         <f t="shared" si="0"/>
         <v>1/16/2024 02:48:00 AM</v>
       </c>
+      <c r="C25">
+        <v>0</v>
+      </c>
       <c r="J25">
         <v>0.39400000000000002</v>
       </c>
@@ -1193,6 +1247,9 @@
         <f t="shared" si="0"/>
         <v>1/16/2024 03:00:00 AM</v>
       </c>
+      <c r="C26">
+        <v>0</v>
+      </c>
       <c r="I26">
         <v>0.39400000000000002</v>
       </c>
@@ -1217,6 +1274,9 @@
         <f t="shared" si="0"/>
         <v>1/16/2024 04:47:00 AM</v>
       </c>
+      <c r="C27">
+        <v>0</v>
+      </c>
       <c r="M27">
         <v>1</v>
       </c>
@@ -1232,6 +1292,9 @@
         <f t="shared" si="0"/>
         <v>1/16/2024 05:00:00 AM</v>
       </c>
+      <c r="C28">
+        <v>0</v>
+      </c>
       <c r="I28">
         <v>0.39400000000000002</v>
       </c>
@@ -1295,6 +1358,9 @@
       <c r="B31" s="14" t="str">
         <f t="shared" si="0"/>
         <v>1/16/2024 06:00:00 AM</v>
+      </c>
+      <c r="C31">
+        <v>0</v>
       </c>
       <c r="I31">
         <v>0.39400000000000002</v>
@@ -1319,6 +1385,9 @@
         <f t="shared" si="0"/>
         <v>1/16/2024 07:00:00 AM</v>
       </c>
+      <c r="C32">
+        <v>0</v>
+      </c>
       <c r="I32">
         <v>0.39400000000000002</v>
       </c>
@@ -1370,6 +1439,9 @@
         <f t="shared" si="0"/>
         <v>1/16/2024 08:27:00 AM</v>
       </c>
+      <c r="C34">
+        <v>0</v>
+      </c>
       <c r="M34">
         <v>1</v>
       </c>
@@ -1385,6 +1457,9 @@
         <f t="shared" si="0"/>
         <v>1/16/2024 09:00:00 AM</v>
       </c>
+      <c r="C35">
+        <v>0</v>
+      </c>
       <c r="I35">
         <v>0.39400000000000002</v>
       </c>
@@ -1448,6 +1523,9 @@
         <f t="shared" si="0"/>
         <v>1/16/2024 10:00:00 AM</v>
       </c>
+      <c r="C38">
+        <v>0</v>
+      </c>
       <c r="H38" s="9"/>
       <c r="I38" s="9">
         <v>0.59099999999999997</v>
@@ -1488,6 +1566,9 @@
       <c r="B40" s="14" t="str">
         <f t="shared" si="0"/>
         <v>1/16/2024 11:00:00 AM</v>
+      </c>
+      <c r="C40">
+        <v>0</v>
       </c>
       <c r="I40">
         <v>0.59099999999999997</v>

</xml_diff>